<commit_message>
solo le queda cerrar lo de que chequee que archivos hay en la nube, y si esta vacio que cree el archivo y si no que lo actualice
</commit_message>
<xml_diff>
--- a/MyHandling Bot/Flights.xlsx
+++ b/MyHandling Bot/Flights.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Regist.(Call sign)</t>
   </si>
@@ -50,97 +50,73 @@
     <t>Reference</t>
   </si>
   <si>
+    <t>ECNBS(GES441S)</t>
+  </si>
+  <si>
+    <t>C68A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>LEBL</t>
+  </si>
+  <si>
+    <t>LEIB (Spain - S)</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>GESTAIR</t>
+  </si>
+  <si>
+    <t>BCN012138</t>
+  </si>
+  <si>
     <t>ECLAE(GES231E)</t>
   </si>
   <si>
     <t>GALX</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>EGAA (United Kingdom)</t>
-  </si>
-  <si>
-    <t>LEBL</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>GESTAIR</t>
-  </si>
-  <si>
-    <t>BCN012146</t>
-  </si>
-  <si>
-    <t>S5BBG(S5BBG)</t>
-  </si>
-  <si>
-    <t>C550</t>
-  </si>
-  <si>
-    <t>LEIB (Spain - S)</t>
-  </si>
-  <si>
-    <t>PHS - Premium Aviation and Handling Services, Soc. U.P. Lda</t>
-  </si>
-  <si>
-    <t>BCN012213</t>
-  </si>
-  <si>
-    <t>N66ZG(N66ZG)</t>
+    <t>LEMD (Spain - S)</t>
+  </si>
+  <si>
+    <t>BCN012186</t>
+  </si>
+  <si>
+    <t>DAWWW(DCS103)</t>
   </si>
   <si>
     <t>GLF6</t>
   </si>
   <si>
-    <t>P</t>
+    <t>EDDS (Germany - S)</t>
+  </si>
+  <si>
+    <t>DC Aviation GmbH</t>
+  </si>
+  <si>
+    <t>BCN012165</t>
+  </si>
+  <si>
+    <t>BCN012112</t>
+  </si>
+  <si>
+    <t>LEPA (Spain - S)</t>
+  </si>
+  <si>
+    <t>EGKB (United Kingdom)</t>
   </si>
   <si>
     <t>LFMN (France - S)</t>
   </si>
   <si>
-    <t>International Trip Planning Services</t>
-  </si>
-  <si>
-    <t>BCN012121</t>
-  </si>
-  <si>
-    <t>ECHYI(GES482Y)</t>
-  </si>
-  <si>
-    <t>F2TH</t>
-  </si>
-  <si>
-    <t>LEMD (Spain - S)</t>
-  </si>
-  <si>
-    <t>BCN012197</t>
-  </si>
-  <si>
-    <t>LEMG (Spain - S)</t>
-  </si>
-  <si>
-    <t>DCFHZ(DCFHZ)</t>
-  </si>
-  <si>
-    <t>E55P</t>
-  </si>
-  <si>
-    <t>EBBR (Belgium - S)</t>
-  </si>
-  <si>
-    <t>DAS Private Jets GmbH</t>
-  </si>
-  <si>
-    <t>BCN012173</t>
-  </si>
-  <si>
-    <t>LIPH (Italy - S)</t>
-  </si>
-  <si>
-    <t>BCN012222</t>
+    <t>BCN012113</t>
+  </si>
+  <si>
+    <t>BCN011974</t>
   </si>
 </sst>
 </file>
@@ -204,17 +180,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.8788423538208" customWidth="1"/>
+    <col min="1" max="1" width="17.8114128112793" customWidth="1"/>
     <col min="2" max="2" width="9.37112331390381" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="10.9916591644287" customWidth="1"/>
     <col min="5" max="5" width="17.2691879272461" customWidth="1"/>
-    <col min="6" max="6" width="22.3169898986816" customWidth="1"/>
-    <col min="7" max="7" width="17.5218849182129" customWidth="1"/>
+    <col min="6" max="6" width="22.1134014129639" customWidth="1"/>
+    <col min="7" max="7" width="22.1134014129639" customWidth="1"/>
     <col min="8" max="8" width="9.140625" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
     <col min="10" max="10" width="9.140625" customWidth="1"/>
-    <col min="11" max="11" width="54.1691017150879" customWidth="1"/>
+    <col min="11" max="11" width="17.6732978820801" customWidth="1"/>
     <col min="12" max="12" width="11.692458152771" customWidth="1"/>
   </cols>
   <sheetData>
@@ -265,13 +241,13 @@
         <v>13</v>
       </c>
       <c r="C2" s="0">
-        <v>16080</v>
+        <v>13971</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="2">
-        <v>44803.3819444444</v>
+        <v>44804.2708333333</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>15</v>
@@ -280,7 +256,7 @@
         <v>16</v>
       </c>
       <c r="H2" s="0">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I2" s="0">
         <v>3</v>
@@ -303,98 +279,98 @@
         <v>21</v>
       </c>
       <c r="C3" s="0">
-        <v>6577</v>
+        <v>16080</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="2">
-        <v>44803.5347222222</v>
+        <v>44804.3611111111</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>22</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" s="0">
         <v>4</v>
       </c>
       <c r="I3" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>17</v>
       </c>
       <c r="K3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0">
+        <v>45177</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2">
+        <v>44804.3819444444</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="0">
-        <v>46991</v>
-      </c>
-      <c r="D4" s="0" t="s">
+      <c r="G4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="0">
+        <v>3</v>
+      </c>
+      <c r="I4" s="0">
+        <v>4</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="2">
-        <v>44803.4513888889</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="0" t="s">
+      <c r="L4" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="H4" s="0">
-        <v>0</v>
-      </c>
-      <c r="I4" s="0">
-        <v>3</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0">
-        <v>16556</v>
+        <v>13971</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="2">
-        <v>44803.5104166667</v>
+        <v>44804.3819444444</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I5" s="0">
         <v>3</v>
@@ -406,15 +382,15 @@
         <v>18</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C6" s="0">
         <v>16080</v>
@@ -423,16 +399,16 @@
         <v>14</v>
       </c>
       <c r="E6" s="2">
-        <v>44803.5</v>
+        <v>44804.3854166667</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H6" s="0">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I6" s="0">
         <v>3</v>
@@ -444,33 +420,33 @@
         <v>18</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="0">
+        <v>13971</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="2">
+        <v>44804.4166666667</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="0">
-        <v>16556</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="2">
-        <v>44803.5381944444</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="H7" s="0">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I7" s="0">
         <v>3</v>
@@ -482,33 +458,33 @@
         <v>18</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C8" s="0">
-        <v>8340</v>
+        <v>16080</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="2">
-        <v>44803.5833333333</v>
+        <v>44804.5833333333</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="H8" s="0">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I8" s="0">
         <v>2</v>
@@ -517,86 +493,86 @@
         <v>17</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C9" s="0">
-        <v>6577</v>
+        <v>13971</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2">
-        <v>44803.7291666667</v>
+        <v>44804.6388888889</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="H9" s="0">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I9" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J9" s="0" t="s">
         <v>17</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C10" s="0">
-        <v>6577</v>
+        <v>45177</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="2">
-        <v>44803.9270833333</v>
+        <v>44804.6666666667</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="H10" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I10" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J10" s="0" t="s">
         <v>17</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>